<commit_message>
debug the item amout 0.5 problem
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -8,9 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GO\專案\go train\WeeklyInventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0135B6FC-E58E-4BF2-B6E1-50E54884F01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
   <si>
     <t>髮圈</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -127,57 +126,64 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>廠商1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>廠商2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>廠商3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>庫存警戒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>404</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>04/17</t>
+  </si>
+  <si>
     <t>4</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>廠商1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>廠商2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>廠商3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>2023/04/03</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>156</t>
-  </si>
-  <si>
-    <t>2023/06/03</t>
+    <t>0.5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,7 +242,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,19 +251,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.5999938962981048"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.5999938962981048"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.3999755851924192"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -274,7 +280,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.5999938962981048"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.3999755851924192"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -290,45 +302,46 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="true" applyAlignment="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment wrapText="true"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -337,7 +350,7 @@
     <cellStyle name="好" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -350,120 +363,120 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
+<theme xmlns="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <themeElements>
+    <clrScheme name="Office">
+      <dk1>
+        <sysClr val="windowText" lastClr="000000"/>
+      </dk1>
+      <lt1>
+        <sysClr val="window" lastClr="FFFFFF"/>
+      </lt1>
+      <dk2>
+        <srgbClr val="44546A"/>
+      </dk2>
+      <lt2>
+        <srgbClr val="E7E6E6"/>
+      </lt2>
+      <accent1>
+        <srgbClr val="5B9BD5"/>
+      </accent1>
+      <accent2>
+        <srgbClr val="ED7D31"/>
+      </accent2>
+      <accent3>
+        <srgbClr val="A5A5A5"/>
+      </accent3>
+      <accent4>
+        <srgbClr val="FFC000"/>
+      </accent4>
+      <accent5>
+        <srgbClr val="4472C4"/>
+      </accent5>
+      <accent6>
+        <srgbClr val="70AD47"/>
+      </accent6>
+      <hlink>
+        <srgbClr val="0563C1"/>
+      </hlink>
+      <folHlink>
+        <srgbClr val="954F72"/>
+      </folHlink>
+    </clrScheme>
+    <fontScheme name="Office">
+      <majorFont>
+        <latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <ea typeface=""/>
+        <cs typeface=""/>
+        <font script="Jpan" typeface="Yu Gothic Light"/>
+        <font script="Hang" typeface="맑은 고딕"/>
+        <font script="Hans" typeface="等线 Light"/>
+        <font script="Hant" typeface="新細明體"/>
+        <font script="Arab" typeface="Times New Roman"/>
+        <font script="Hebr" typeface="Times New Roman"/>
+        <font script="Thai" typeface="Tahoma"/>
+        <font script="Ethi" typeface="Nyala"/>
+        <font script="Beng" typeface="Vrinda"/>
+        <font script="Gujr" typeface="Shruti"/>
+        <font script="Khmr" typeface="MoolBoran"/>
+        <font script="Knda" typeface="Tunga"/>
+        <font script="Guru" typeface="Raavi"/>
+        <font script="Cans" typeface="Euphemia"/>
+        <font script="Cher" typeface="Plantagenet Cherokee"/>
+        <font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <font script="Tibt" typeface="Microsoft Himalaya"/>
+        <font script="Thaa" typeface="MV Boli"/>
+        <font script="Deva" typeface="Mangal"/>
+        <font script="Telu" typeface="Gautami"/>
+        <font script="Taml" typeface="Latha"/>
+        <font script="Syrc" typeface="Estrangelo Edessa"/>
+        <font script="Orya" typeface="Kalinga"/>
+        <font script="Mlym" typeface="Kartika"/>
+        <font script="Laoo" typeface="DokChampa"/>
+        <font script="Sinh" typeface="Iskoola Pota"/>
+        <font script="Mong" typeface="Mongolian Baiti"/>
+        <font script="Viet" typeface="Times New Roman"/>
+        <font script="Uigh" typeface="Microsoft Uighur"/>
+        <font script="Geor" typeface="Sylfaen"/>
+      </majorFont>
+      <minorFont>
+        <latin typeface="Calibri" panose="020F0502020204030204"/>
+        <ea typeface=""/>
+        <cs typeface=""/>
+        <font script="Jpan" typeface="Yu Gothic"/>
+        <font script="Hang" typeface="맑은 고딕"/>
+        <font script="Hans" typeface="等线"/>
+        <font script="Hant" typeface="新細明體"/>
+        <font script="Arab" typeface="Arial"/>
+        <font script="Hebr" typeface="Arial"/>
+        <font script="Thai" typeface="Tahoma"/>
+        <font script="Ethi" typeface="Nyala"/>
+        <font script="Beng" typeface="Vrinda"/>
+        <font script="Gujr" typeface="Shruti"/>
+        <font script="Khmr" typeface="DaunPenh"/>
+        <font script="Knda" typeface="Tunga"/>
+        <font script="Guru" typeface="Raavi"/>
+        <font script="Cans" typeface="Euphemia"/>
+        <font script="Cher" typeface="Plantagenet Cherokee"/>
+        <font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <font script="Tibt" typeface="Microsoft Himalaya"/>
+        <font script="Thaa" typeface="MV Boli"/>
+        <font script="Deva" typeface="Mangal"/>
+        <font script="Telu" typeface="Gautami"/>
+        <font script="Taml" typeface="Latha"/>
+        <font script="Syrc" typeface="Estrangelo Edessa"/>
+        <font script="Orya" typeface="Kalinga"/>
+        <font script="Mlym" typeface="Kartika"/>
+        <font script="Laoo" typeface="DokChampa"/>
+        <font script="Sinh" typeface="Iskoola Pota"/>
+        <font script="Mong" typeface="Mongolian Baiti"/>
+        <font script="Viet" typeface="Arial"/>
+        <font script="Uigh" typeface="Microsoft Uighur"/>
+        <font script="Geor" typeface="Sylfaen"/>
+      </minorFont>
+    </fontScheme>
+    <fmtScheme name="Office">
+      <fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -519,8 +532,8 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
+      </fillStyleLst>
+      <lnStyleLst>
         <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -542,8 +555,8 @@
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
+      </lnStyleLst>
+      <effectStyleLst>
         <a:effectStyle>
           <a:effectLst/>
         </a:effectStyle>
@@ -559,8 +572,8 @@
             </a:outerShdw>
           </a:effectLst>
         </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
+      </effectStyleLst>
+      <bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -597,17 +610,17 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
+      </bgFillStyleLst>
+    </fmtScheme>
+  </themeElements>
+  <objectDefaults/>
+  <extraClrSchemeLst/>
+  <extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
       <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
-  </a:extLst>
-</a:theme>
+  </extLst>
+</theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -615,34 +628,34 @@
   <sheetPr codeName="工作表1"/>
   <dimension ref="A1:V40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" customWidth="1"/>
-    <col min="20" max="20" width="12.5703125" customWidth="1"/>
+    <col customWidth="true" max="1" min="1" width="18.140625"/>
+    <col customWidth="true" max="2" min="2" width="11.42578125"/>
+    <col bestFit="true" customWidth="true" max="4" min="3" width="11.5703125"/>
+    <col bestFit="true" customWidth="true" max="5" min="5" width="10"/>
+    <col bestFit="true" customWidth="true" max="6" min="6" width="9.42578125"/>
+    <col bestFit="true" customWidth="true" max="10" min="10" width="10"/>
+    <col customWidth="true" max="18" min="18" width="9.140625"/>
+    <col customWidth="true" max="20" min="20" width="12.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22">
       <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:22" ht="19.5" customHeight="true">
       <c r="B2" t="s">
         <v>17</v>
       </c>
@@ -650,39 +663,44 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="21.75" customHeight="true">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C3" s="18" t="str">
         <f>DATEDIF(B3, D3, "d")&amp;"天"</f>
-        <v>59天</v>
+        <v>61天</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="19" t="s">
+        <v>30</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="J3" s="15"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="C4" s="7">
         <f>IF(AND(B4&lt;&gt;"", D4&lt;&gt;""), B4-D4, "")</f>
         <v>-400</v>
       </c>
-      <c r="D4" s="7">
-        <v>404</v>
-      </c>
-      <c r="E4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="7" t="str">
+        <f>IF(D4&lt;3, "叫一箱貨", "不用叫貨")</f>
+        <v>不用叫貨</v>
+      </c>
       <c r="F4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -695,21 +713,24 @@
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C5" s="7">
         <f t="shared" ref="C5:C19" si="0">IF(AND(B5&lt;&gt;"", D5&lt;&gt;""), B5-D5, "")</f>
         <v>0</v>
       </c>
-      <c r="D5" s="7">
-        <v>8</v>
-      </c>
-      <c r="E5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="7" t="str">
+        <f t="shared" ref="E5" si="1">IF(D5&lt;3, "叫一箱貨", "不用叫貨")</f>
+        <v>不用叫貨</v>
+      </c>
       <c r="F5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -722,7 +743,7 @@
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -733,10 +754,13 @@
         <f t="shared" si="0"/>
         <v>-3</v>
       </c>
-      <c r="D6" s="7">
-        <v>3</v>
-      </c>
-      <c r="E6" s="7"/>
+      <c r="D6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="7" t="str">
+        <f>IF(D6&lt;=2, "叫一箱貨", "不用叫貨")</f>
+        <v>不用叫貨</v>
+      </c>
       <c r="F6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -749,7 +773,7 @@
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -760,10 +784,13 @@
         <f t="shared" si="0"/>
         <v>-7</v>
       </c>
-      <c r="D7" s="7">
-        <v>12</v>
-      </c>
-      <c r="E7" s="7"/>
+      <c r="D7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="7" t="str">
+        <f>IF(D7&lt;=5, "叫兩箱貨", IF(D7&lt;15, "叫一箱貨", "不用叫貨"))</f>
+        <v>叫一箱貨</v>
+      </c>
       <c r="F7" s="7"/>
       <c r="H7" s="17"/>
       <c r="I7" s="7"/>
@@ -776,21 +803,24 @@
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D8" s="7">
-        <v>7</v>
-      </c>
-      <c r="E8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="7" t="str">
+        <f>IF(D8&lt;=2, "叫一箱貨", "不用叫貨")</f>
+        <v>不用叫貨</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
@@ -803,7 +833,7 @@
       <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -814,10 +844,13 @@
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="D9" s="7">
-        <v>6</v>
-      </c>
-      <c r="E9" s="7"/>
+      <c r="D9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="7" t="str">
+        <f>IF(D9&lt;=6, "叫兩箱貨", IF(D9&lt;12, "叫一箱貨", "不用叫貨"))</f>
+        <v>叫兩箱貨</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -830,21 +863,24 @@
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D10" s="7">
-        <v>9</v>
-      </c>
-      <c r="E10" s="7"/>
+      <c r="D10" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="7" t="str">
+        <f>IF(D10&lt;=5, "叫一箱貨", "不用叫貨")</f>
+        <v>不用叫貨</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -857,7 +893,7 @@
       <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -866,10 +902,12 @@
       </c>
       <c r="C11" s="7" t="str">
         <f t="shared" si="0"/>
-        <v/>
       </c>
       <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="E11" s="7" t="str">
+        <f>IF(D11&lt;=7, "叫一箱貨", "不用叫貨")</f>
+        <v>叫一箱貨</v>
+      </c>
       <c r="F11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
@@ -883,7 +921,7 @@
       <c r="Q11" s="7"/>
       <c r="R11" s="12"/>
     </row>
-    <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="15.75" customHeight="true">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -892,10 +930,12 @@
       </c>
       <c r="C12" s="7" t="str">
         <f t="shared" si="0"/>
-        <v/>
       </c>
       <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="E12" s="7" t="str">
+        <f>IF(D12&lt;=8, "叫一箱貨", "不用叫貨")</f>
+        <v>叫一箱貨</v>
+      </c>
       <c r="F12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
@@ -911,7 +951,7 @@
       <c r="T12" s="14"/>
       <c r="V12" s="14"/>
     </row>
-    <row r="13" spans="1:22" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="16.5">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
@@ -920,10 +960,12 @@
       </c>
       <c r="C13" s="7" t="str">
         <f t="shared" si="0"/>
-        <v/>
       </c>
       <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="E13" s="7" t="str">
+        <f>IF(D13&lt;1, "叫一箱貨", "不用叫貨")</f>
+        <v>叫一箱貨</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
@@ -937,7 +979,7 @@
       <c r="Q13" s="7"/>
       <c r="R13" s="13"/>
     </row>
-    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="15.75" customHeight="true">
       <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
@@ -946,10 +988,12 @@
       </c>
       <c r="C14" s="7" t="str">
         <f t="shared" si="0"/>
-        <v/>
       </c>
       <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+      <c r="E14" s="7" t="str">
+        <f t="shared" ref="E14:E16" si="2">IF(D14&lt;1, "叫一箱貨", "不用叫貨")</f>
+        <v>叫一箱貨</v>
+      </c>
       <c r="F14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
@@ -963,7 +1007,7 @@
       <c r="Q14" s="7"/>
       <c r="R14" s="13"/>
     </row>
-    <row r="15" spans="1:22" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="16.5">
       <c r="A15" s="4" t="s">
         <v>3</v>
       </c>
@@ -972,10 +1016,12 @@
       </c>
       <c r="C15" s="7" t="str">
         <f t="shared" si="0"/>
-        <v/>
       </c>
       <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="E15" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>叫一箱貨</v>
+      </c>
       <c r="F15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
@@ -989,7 +1035,7 @@
       <c r="Q15" s="7"/>
       <c r="R15" s="13"/>
     </row>
-    <row r="16" spans="1:22" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="16.5">
       <c r="A16" s="4" t="s">
         <v>2</v>
       </c>
@@ -998,10 +1044,12 @@
       </c>
       <c r="C16" s="7" t="str">
         <f t="shared" si="0"/>
-        <v/>
       </c>
       <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+      <c r="E16" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>叫一箱貨</v>
+      </c>
       <c r="F16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
@@ -1015,21 +1063,24 @@
       <c r="Q16" s="7"/>
       <c r="R16" s="13"/>
     </row>
-    <row r="17" spans="1:18" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="16.5">
       <c r="A17" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D17" s="7">
-        <v>2</v>
-      </c>
-      <c r="E17" s="7"/>
+      <c r="D17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="7" t="str">
+        <f>IF(D17&lt;=2, "叫兩袋貨", "不用叫貨")</f>
+        <v>叫兩袋貨</v>
+      </c>
       <c r="F17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
@@ -1043,7 +1094,7 @@
       <c r="Q17" s="7"/>
       <c r="R17" s="13"/>
     </row>
-    <row r="18" spans="1:18" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="16.5">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -1052,7 +1103,6 @@
       </c>
       <c r="C18" s="7" t="str">
         <f t="shared" si="0"/>
-        <v/>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -1069,7 +1119,7 @@
       <c r="Q18" s="7"/>
       <c r="R18" s="13"/>
     </row>
-    <row r="19" spans="1:18" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="16.5">
       <c r="A19" s="10" t="s">
         <v>0</v>
       </c>
@@ -1078,7 +1128,6 @@
       </c>
       <c r="C19" s="7" t="str">
         <f t="shared" si="0"/>
-        <v/>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -1095,7 +1144,7 @@
       <c r="P19" s="9"/>
       <c r="R19" s="13"/>
     </row>
-    <row r="20" spans="1:18" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="16.5">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -1109,8 +1158,8 @@
       <c r="P20" s="5"/>
       <c r="R20" s="13"/>
     </row>
-    <row r="21" spans="1:18" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+    <row r="21" spans="1:18" ht="16.5">
+      <c r="A21" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="11"/>
@@ -1118,13 +1167,13 @@
       <c r="P21" s="5"/>
       <c r="R21" s="13"/>
     </row>
-    <row r="22" spans="1:18" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
+    <row r="22" spans="1:18" ht="16.5">
+      <c r="A22" s="20"/>
       <c r="C22" s="11"/>
       <c r="P22" s="5"/>
       <c r="R22" s="13"/>
     </row>
-    <row r="23" spans="1:18" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="16.5">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1134,28 +1183,28 @@
       <c r="P23" s="5"/>
       <c r="R23" s="13"/>
     </row>
-    <row r="24" spans="1:18" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" ht="16.5">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="7"/>
       <c r="R24" s="13"/>
     </row>
-    <row r="25" spans="1:18" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" ht="16.5">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B25" s="7"/>
       <c r="R25" s="13"/>
     </row>
-    <row r="26" spans="1:18" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="16.5">
       <c r="A26" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B26" s="7"/>
       <c r="R26" s="13"/>
     </row>
-    <row r="27" spans="1:18" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" ht="16.5">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
@@ -1164,14 +1213,14 @@
       </c>
       <c r="R27" s="13"/>
     </row>
-    <row r="28" spans="1:18" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="16.5">
       <c r="A28" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B28" s="7"/>
       <c r="R28" s="13"/>
     </row>
-    <row r="29" spans="1:18" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" ht="16.5">
       <c r="A29" s="3" t="s">
         <v>10</v>
       </c>
@@ -1180,7 +1229,7 @@
       </c>
       <c r="R29" s="13"/>
     </row>
-    <row r="30" spans="1:18" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" ht="16.5">
       <c r="A30" s="3" t="s">
         <v>11</v>
       </c>
@@ -1189,21 +1238,21 @@
       </c>
       <c r="R30" s="13"/>
     </row>
-    <row r="31" spans="1:18" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="16.5">
       <c r="A31" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B31" s="7"/>
       <c r="R31" s="13"/>
     </row>
-    <row r="32" spans="1:18" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" ht="16.5">
       <c r="A32" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B32" s="7"/>
       <c r="R32" s="13"/>
     </row>
-    <row r="33" spans="1:18" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="16.5">
       <c r="A33" s="3" t="s">
         <v>21</v>
       </c>
@@ -1212,45 +1261,45 @@
       </c>
       <c r="R33" s="13"/>
     </row>
-    <row r="34" spans="1:18" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" ht="16.5">
       <c r="A34" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B34" s="7"/>
       <c r="R34" s="13"/>
     </row>
-    <row r="35" spans="1:18" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="16.5">
       <c r="A35" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B35" s="7"/>
       <c r="R35" s="13"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18">
       <c r="A36" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B36" s="7"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18">
       <c r="A37" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B37" s="7"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18">
       <c r="A38" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B38" s="7"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18">
       <c r="A39" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B39" s="7"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18">
       <c r="A40" s="10" t="s">
         <v>0</v>
       </c>
@@ -1261,7 +1310,69 @@
     <mergeCell ref="A21:A22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="E5:E6">
+    <cfRule type="iconSet" priority="6">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10:E12">
+    <cfRule type="iconSet" priority="3">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup r:id="rId1" orientation="portrait" paperSize="9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="4" id="{838DC943-6D8B-4C98-B78A-2300BB56AFD6}">
+            <x14:iconSet iconSet="3Symbols" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>3</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>E5:E6</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="2" id="{DD668BCF-FFD8-4EFB-B432-7BF53355462A}">
+            <x14:iconSet iconSet="3Symbols" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>3</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>E10:E12</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>